<commit_message>
ok na yung delete product
</commit_message>
<xml_diff>
--- a/CSSECDV - Case Study 2 Access Matrix.xlsx
+++ b/CSSECDV - Case Study 2 Access Matrix.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="BrfnfJyTxpomh3LMP599QuDvyUH6GMBze2qAe774mzA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="TTNb4kjHMGn8yDiT0s5YdFM115FBmGyKrzDdH1fQgu0="/>
     </ext>
   </extLst>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
     <t>ACCESS MATRIX</t>
   </si>
@@ -57,10 +57,19 @@
     <t>User - Search</t>
   </si>
   <si>
-    <t>User - Logs</t>
-  </si>
-  <si>
-    <t>User - Re-enabling Disabled Accounts</t>
+    <t>User - Edit Role</t>
+  </si>
+  <si>
+    <t>User - Change Password</t>
+  </si>
+  <si>
+    <t>User - Delete User</t>
+  </si>
+  <si>
+    <t>User - View Logs</t>
+  </si>
+  <si>
+    <t>User - Lock/Unlock Accounts</t>
   </si>
   <si>
     <t>User - View Own Purchase History</t>
@@ -549,7 +558,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border/>
     <border>
       <left/>
@@ -680,6 +689,11 @@
       </bottom>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+    </border>
+    <border>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -735,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -804,10 +818,13 @@
     <xf borderId="16" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="13" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -829,25 +846,25 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="14" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="22" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1072,7 +1089,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.71"/>
-    <col customWidth="1" min="2" max="107" width="20.86"/>
+    <col customWidth="1" min="2" max="110" width="20.86"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -1184,7 +1201,10 @@
       <c r="CZ1" s="2"/>
       <c r="DA1" s="2"/>
       <c r="DB1" s="2"/>
-      <c r="DC1" s="3"/>
+      <c r="DC1" s="2"/>
+      <c r="DD1" s="2"/>
+      <c r="DE1" s="2"/>
+      <c r="DF1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
@@ -1220,13 +1240,13 @@
       <c r="K2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="O2" s="6" t="s">
@@ -1505,13 +1525,22 @@
       <c r="DB2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="DC2" s="8" t="s">
+      <c r="DC2" s="6" t="s">
         <v>107</v>
+      </c>
+      <c r="DD2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="DE2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="DF2" s="8" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
@@ -1618,11 +1647,14 @@
       <c r="CZ3" s="11"/>
       <c r="DA3" s="11"/>
       <c r="DB3" s="11"/>
-      <c r="DC3" s="12"/>
+      <c r="DC3" s="11"/>
+      <c r="DD3" s="11"/>
+      <c r="DE3" s="11"/>
+      <c r="DF3" s="12"/>
     </row>
     <row r="4" ht="19.5" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="11"/>
@@ -1729,22 +1761,25 @@
       <c r="CZ4" s="11"/>
       <c r="DA4" s="11"/>
       <c r="DB4" s="11"/>
-      <c r="DC4" s="12"/>
+      <c r="DC4" s="11"/>
+      <c r="DD4" s="11"/>
+      <c r="DE4" s="11"/>
+      <c r="DF4" s="12"/>
     </row>
     <row r="5" ht="49.5" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="16"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
@@ -1840,27 +1875,30 @@
       <c r="CZ5" s="11"/>
       <c r="DA5" s="11"/>
       <c r="DB5" s="11"/>
-      <c r="DC5" s="12"/>
+      <c r="DC5" s="11"/>
+      <c r="DD5" s="11"/>
+      <c r="DE5" s="11"/>
+      <c r="DF5" s="12"/>
     </row>
     <row r="6" ht="49.5" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="16"/>
       <c r="D6" s="19" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -1953,27 +1991,30 @@
       <c r="CZ6" s="11"/>
       <c r="DA6" s="11"/>
       <c r="DB6" s="11"/>
-      <c r="DC6" s="12"/>
+      <c r="DC6" s="11"/>
+      <c r="DD6" s="11"/>
+      <c r="DE6" s="11"/>
+      <c r="DF6" s="12"/>
     </row>
     <row r="7" ht="49.5" customHeight="1">
       <c r="A7" s="20" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="16"/>
       <c r="D7" s="19" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="16"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -2066,934 +2107,961 @@
       <c r="CZ7" s="11"/>
       <c r="DA7" s="11"/>
       <c r="DB7" s="11"/>
-      <c r="DC7" s="12"/>
+      <c r="DC7" s="11"/>
+      <c r="DD7" s="11"/>
+      <c r="DE7" s="11"/>
+      <c r="DF7" s="12"/>
     </row>
     <row r="8" ht="49.5" customHeight="1">
       <c r="A8" s="21" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="24"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="24"/>
-      <c r="AG8" s="24"/>
-      <c r="AH8" s="24"/>
-      <c r="AI8" s="24"/>
-      <c r="AJ8" s="24"/>
-      <c r="AK8" s="24"/>
-      <c r="AL8" s="24"/>
-      <c r="AM8" s="24"/>
-      <c r="AN8" s="24"/>
-      <c r="AO8" s="24"/>
-      <c r="AP8" s="24"/>
-      <c r="AQ8" s="24"/>
-      <c r="AR8" s="24"/>
-      <c r="AS8" s="24"/>
-      <c r="AT8" s="24"/>
-      <c r="AU8" s="24"/>
-      <c r="AV8" s="24"/>
-      <c r="AW8" s="24"/>
-      <c r="AX8" s="24"/>
-      <c r="AY8" s="24"/>
-      <c r="AZ8" s="24"/>
-      <c r="BA8" s="24"/>
-      <c r="BB8" s="24"/>
-      <c r="BC8" s="24"/>
-      <c r="BD8" s="24"/>
-      <c r="BE8" s="24"/>
-      <c r="BF8" s="24"/>
-      <c r="BG8" s="24"/>
-      <c r="BH8" s="24"/>
-      <c r="BI8" s="24"/>
-      <c r="BJ8" s="24"/>
-      <c r="BK8" s="24"/>
-      <c r="BL8" s="24"/>
-      <c r="BM8" s="24"/>
-      <c r="BN8" s="24"/>
-      <c r="BO8" s="24"/>
-      <c r="BP8" s="24"/>
-      <c r="BQ8" s="24"/>
-      <c r="BR8" s="24"/>
-      <c r="BS8" s="24"/>
-      <c r="BT8" s="24"/>
-      <c r="BU8" s="24"/>
-      <c r="BV8" s="24"/>
-      <c r="BW8" s="24"/>
-      <c r="BX8" s="24"/>
-      <c r="BY8" s="24"/>
-      <c r="BZ8" s="24"/>
-      <c r="CA8" s="24"/>
-      <c r="CB8" s="24"/>
-      <c r="CC8" s="24"/>
-      <c r="CD8" s="24"/>
-      <c r="CE8" s="24"/>
-      <c r="CF8" s="24"/>
-      <c r="CG8" s="24"/>
-      <c r="CH8" s="24"/>
-      <c r="CI8" s="24"/>
-      <c r="CJ8" s="24"/>
-      <c r="CK8" s="24"/>
-      <c r="CL8" s="24"/>
-      <c r="CM8" s="24"/>
-      <c r="CN8" s="24"/>
-      <c r="CO8" s="24"/>
-      <c r="CP8" s="24"/>
-      <c r="CQ8" s="24"/>
-      <c r="CR8" s="24"/>
-      <c r="CS8" s="24"/>
-      <c r="CT8" s="24"/>
-      <c r="CU8" s="24"/>
-      <c r="CV8" s="24"/>
-      <c r="CW8" s="24"/>
-      <c r="CX8" s="24"/>
-      <c r="CY8" s="24"/>
-      <c r="CZ8" s="24"/>
-      <c r="DA8" s="24"/>
-      <c r="DB8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="25"/>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="25"/>
+      <c r="AF8" s="25"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="25"/>
+      <c r="AJ8" s="25"/>
+      <c r="AK8" s="25"/>
+      <c r="AL8" s="25"/>
+      <c r="AM8" s="25"/>
+      <c r="AN8" s="25"/>
+      <c r="AO8" s="25"/>
+      <c r="AP8" s="25"/>
+      <c r="AQ8" s="25"/>
+      <c r="AR8" s="25"/>
+      <c r="AS8" s="25"/>
+      <c r="AT8" s="25"/>
+      <c r="AU8" s="25"/>
+      <c r="AV8" s="25"/>
+      <c r="AW8" s="25"/>
+      <c r="AX8" s="25"/>
+      <c r="AY8" s="25"/>
+      <c r="AZ8" s="25"/>
+      <c r="BA8" s="25"/>
+      <c r="BB8" s="25"/>
+      <c r="BC8" s="25"/>
+      <c r="BD8" s="25"/>
+      <c r="BE8" s="25"/>
+      <c r="BF8" s="25"/>
+      <c r="BG8" s="25"/>
+      <c r="BH8" s="25"/>
+      <c r="BI8" s="25"/>
+      <c r="BJ8" s="25"/>
+      <c r="BK8" s="25"/>
+      <c r="BL8" s="25"/>
+      <c r="BM8" s="25"/>
+      <c r="BN8" s="25"/>
+      <c r="BO8" s="25"/>
+      <c r="BP8" s="25"/>
+      <c r="BQ8" s="25"/>
+      <c r="BR8" s="25"/>
+      <c r="BS8" s="25"/>
+      <c r="BT8" s="25"/>
+      <c r="BU8" s="25"/>
+      <c r="BV8" s="25"/>
+      <c r="BW8" s="25"/>
+      <c r="BX8" s="25"/>
+      <c r="BY8" s="25"/>
+      <c r="BZ8" s="25"/>
+      <c r="CA8" s="25"/>
+      <c r="CB8" s="25"/>
+      <c r="CC8" s="25"/>
+      <c r="CD8" s="25"/>
+      <c r="CE8" s="25"/>
+      <c r="CF8" s="25"/>
+      <c r="CG8" s="25"/>
+      <c r="CH8" s="25"/>
+      <c r="CI8" s="25"/>
+      <c r="CJ8" s="25"/>
+      <c r="CK8" s="25"/>
+      <c r="CL8" s="25"/>
+      <c r="CM8" s="25"/>
+      <c r="CN8" s="25"/>
+      <c r="CO8" s="25"/>
+      <c r="CP8" s="25"/>
+      <c r="CQ8" s="25"/>
+      <c r="CR8" s="25"/>
+      <c r="CS8" s="25"/>
+      <c r="CT8" s="25"/>
+      <c r="CU8" s="25"/>
+      <c r="CV8" s="25"/>
+      <c r="CW8" s="25"/>
+      <c r="CX8" s="25"/>
+      <c r="CY8" s="25"/>
+      <c r="CZ8" s="25"/>
+      <c r="DA8" s="25"/>
+      <c r="DB8" s="25"/>
       <c r="DC8" s="25"/>
+      <c r="DD8" s="25"/>
+      <c r="DE8" s="25"/>
+      <c r="DF8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="26"/>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
-      <c r="AH9" s="26"/>
-      <c r="AI9" s="26"/>
-      <c r="AJ9" s="26"/>
-      <c r="AK9" s="26"/>
-      <c r="AL9" s="26"/>
-      <c r="AM9" s="26"/>
-      <c r="AN9" s="26"/>
-      <c r="AO9" s="26"/>
-      <c r="AP9" s="26"/>
-      <c r="AQ9" s="26"/>
-      <c r="AR9" s="26"/>
-      <c r="AS9" s="26"/>
-      <c r="AT9" s="26"/>
-      <c r="AU9" s="26"/>
-      <c r="AV9" s="26"/>
-      <c r="AW9" s="26"/>
-      <c r="AX9" s="26"/>
-      <c r="AY9" s="26"/>
-      <c r="AZ9" s="26"/>
-      <c r="BA9" s="26"/>
-      <c r="BB9" s="26"/>
-      <c r="BC9" s="26"/>
-      <c r="BD9" s="26"/>
-      <c r="BE9" s="26"/>
-      <c r="BF9" s="26"/>
-      <c r="BG9" s="26"/>
-      <c r="BH9" s="26"/>
-      <c r="BI9" s="26"/>
-      <c r="BJ9" s="26"/>
-      <c r="BK9" s="26"/>
-      <c r="BL9" s="26"/>
-      <c r="BM9" s="26"/>
-      <c r="BN9" s="26"/>
-      <c r="BO9" s="26"/>
-      <c r="BP9" s="26"/>
-      <c r="BQ9" s="26"/>
-      <c r="BR9" s="26"/>
-      <c r="BS9" s="26"/>
-      <c r="BT9" s="26"/>
-      <c r="BU9" s="26"/>
-      <c r="BV9" s="26"/>
-      <c r="BW9" s="26"/>
-      <c r="BX9" s="26"/>
-      <c r="BY9" s="26"/>
-      <c r="BZ9" s="26"/>
-      <c r="CA9" s="26"/>
-      <c r="CB9" s="26"/>
-      <c r="CC9" s="26"/>
-      <c r="CD9" s="26"/>
-      <c r="CE9" s="26"/>
-      <c r="CF9" s="26"/>
-      <c r="CG9" s="26"/>
-      <c r="CH9" s="26"/>
-      <c r="CI9" s="26"/>
-      <c r="CJ9" s="26"/>
-      <c r="CK9" s="26"/>
-      <c r="CL9" s="26"/>
-      <c r="CM9" s="26"/>
-      <c r="CN9" s="26"/>
-      <c r="CO9" s="26"/>
-      <c r="CP9" s="26"/>
-      <c r="CQ9" s="26"/>
-      <c r="CR9" s="26"/>
-      <c r="CS9" s="26"/>
-      <c r="CT9" s="26"/>
-      <c r="CU9" s="26"/>
-      <c r="CV9" s="26"/>
-      <c r="CW9" s="26"/>
-      <c r="CX9" s="26"/>
-      <c r="CY9" s="26"/>
-      <c r="CZ9" s="26"/>
-      <c r="DA9" s="26"/>
-      <c r="DB9" s="26"/>
-      <c r="DC9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="27"/>
+      <c r="AI9" s="27"/>
+      <c r="AJ9" s="27"/>
+      <c r="AK9" s="27"/>
+      <c r="AL9" s="27"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="27"/>
+      <c r="AP9" s="27"/>
+      <c r="AQ9" s="27"/>
+      <c r="AR9" s="27"/>
+      <c r="AS9" s="27"/>
+      <c r="AT9" s="27"/>
+      <c r="AU9" s="27"/>
+      <c r="AV9" s="27"/>
+      <c r="AW9" s="27"/>
+      <c r="AX9" s="27"/>
+      <c r="AY9" s="27"/>
+      <c r="AZ9" s="27"/>
+      <c r="BA9" s="27"/>
+      <c r="BB9" s="27"/>
+      <c r="BC9" s="27"/>
+      <c r="BD9" s="27"/>
+      <c r="BE9" s="27"/>
+      <c r="BF9" s="27"/>
+      <c r="BG9" s="27"/>
+      <c r="BH9" s="27"/>
+      <c r="BI9" s="27"/>
+      <c r="BJ9" s="27"/>
+      <c r="BK9" s="27"/>
+      <c r="BL9" s="27"/>
+      <c r="BM9" s="27"/>
+      <c r="BN9" s="27"/>
+      <c r="BO9" s="27"/>
+      <c r="BP9" s="27"/>
+      <c r="BQ9" s="27"/>
+      <c r="BR9" s="27"/>
+      <c r="BS9" s="27"/>
+      <c r="BT9" s="27"/>
+      <c r="BU9" s="27"/>
+      <c r="BV9" s="27"/>
+      <c r="BW9" s="27"/>
+      <c r="BX9" s="27"/>
+      <c r="BY9" s="27"/>
+      <c r="BZ9" s="27"/>
+      <c r="CA9" s="27"/>
+      <c r="CB9" s="27"/>
+      <c r="CC9" s="27"/>
+      <c r="CD9" s="27"/>
+      <c r="CE9" s="27"/>
+      <c r="CF9" s="27"/>
+      <c r="CG9" s="27"/>
+      <c r="CH9" s="27"/>
+      <c r="CI9" s="27"/>
+      <c r="CJ9" s="27"/>
+      <c r="CK9" s="27"/>
+      <c r="CL9" s="27"/>
+      <c r="CM9" s="27"/>
+      <c r="CN9" s="27"/>
+      <c r="CO9" s="27"/>
+      <c r="CP9" s="27"/>
+      <c r="CQ9" s="27"/>
+      <c r="CR9" s="27"/>
+      <c r="CS9" s="27"/>
+      <c r="CT9" s="27"/>
+      <c r="CU9" s="27"/>
+      <c r="CV9" s="27"/>
+      <c r="CW9" s="27"/>
+      <c r="CX9" s="27"/>
+      <c r="CY9" s="27"/>
+      <c r="CZ9" s="27"/>
+      <c r="DA9" s="27"/>
+      <c r="DB9" s="27"/>
+      <c r="DC9" s="27"/>
+      <c r="DD9" s="27"/>
+      <c r="DE9" s="27"/>
+      <c r="DF9" s="27"/>
     </row>
     <row r="10" ht="45.0" customHeight="1">
-      <c r="A10" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="28" t="s">
+      <c r="A10" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
-      <c r="AB10" s="29"/>
-      <c r="AC10" s="29"/>
-      <c r="AD10" s="29"/>
-      <c r="AE10" s="29"/>
-      <c r="AF10" s="29"/>
-      <c r="AG10" s="29"/>
-      <c r="AH10" s="29"/>
-      <c r="AI10" s="29"/>
-      <c r="AJ10" s="29"/>
-      <c r="AK10" s="29"/>
-      <c r="AL10" s="29"/>
-      <c r="AM10" s="29"/>
-      <c r="AN10" s="29"/>
-      <c r="AO10" s="29"/>
-      <c r="AP10" s="29"/>
-      <c r="AQ10" s="29"/>
-      <c r="AR10" s="29"/>
-      <c r="AS10" s="29"/>
-      <c r="AT10" s="29"/>
-      <c r="AU10" s="29"/>
-      <c r="AV10" s="29"/>
-      <c r="AW10" s="29"/>
-      <c r="AX10" s="29"/>
-      <c r="AY10" s="29"/>
-      <c r="AZ10" s="29"/>
-      <c r="BA10" s="29"/>
-      <c r="BB10" s="29"/>
-      <c r="BC10" s="29"/>
-      <c r="BD10" s="29"/>
-      <c r="BE10" s="29"/>
-      <c r="BF10" s="29"/>
-      <c r="BG10" s="29"/>
-      <c r="BH10" s="29"/>
-      <c r="BI10" s="29"/>
-      <c r="BJ10" s="29"/>
-      <c r="BK10" s="29"/>
-      <c r="BL10" s="29"/>
-      <c r="BM10" s="29"/>
-      <c r="BN10" s="29"/>
-      <c r="BO10" s="29"/>
-      <c r="BP10" s="29"/>
-      <c r="BQ10" s="29"/>
-      <c r="BR10" s="29"/>
-      <c r="BS10" s="29"/>
-      <c r="BT10" s="29"/>
-      <c r="BU10" s="29"/>
-      <c r="BV10" s="29"/>
-      <c r="BW10" s="29"/>
-      <c r="BX10" s="29"/>
-      <c r="BY10" s="29"/>
-      <c r="BZ10" s="29"/>
-      <c r="CA10" s="29"/>
-      <c r="CB10" s="29"/>
-      <c r="CC10" s="29"/>
-      <c r="CD10" s="29"/>
-      <c r="CE10" s="29"/>
-      <c r="CF10" s="29"/>
-      <c r="CG10" s="29"/>
-      <c r="CH10" s="29"/>
-      <c r="CI10" s="29"/>
-      <c r="CJ10" s="29"/>
-      <c r="CK10" s="29"/>
-      <c r="CL10" s="29"/>
-      <c r="CM10" s="29"/>
-      <c r="CN10" s="29"/>
-      <c r="CO10" s="29"/>
-      <c r="CP10" s="29"/>
-      <c r="CQ10" s="29"/>
-      <c r="CR10" s="29"/>
-      <c r="CS10" s="29"/>
-      <c r="CT10" s="29"/>
-      <c r="CU10" s="29"/>
-      <c r="CV10" s="29"/>
-      <c r="CW10" s="29"/>
-      <c r="CX10" s="29"/>
-      <c r="CY10" s="29"/>
-      <c r="CZ10" s="29"/>
-      <c r="DA10" s="29"/>
-      <c r="DB10" s="29"/>
-      <c r="DC10" s="29"/>
+      <c r="B10" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="30"/>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="30"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="30"/>
+      <c r="AM10" s="30"/>
+      <c r="AN10" s="30"/>
+      <c r="AO10" s="30"/>
+      <c r="AP10" s="30"/>
+      <c r="AQ10" s="30"/>
+      <c r="AR10" s="30"/>
+      <c r="AS10" s="30"/>
+      <c r="AT10" s="30"/>
+      <c r="AU10" s="30"/>
+      <c r="AV10" s="30"/>
+      <c r="AW10" s="30"/>
+      <c r="AX10" s="30"/>
+      <c r="AY10" s="30"/>
+      <c r="AZ10" s="30"/>
+      <c r="BA10" s="30"/>
+      <c r="BB10" s="30"/>
+      <c r="BC10" s="30"/>
+      <c r="BD10" s="30"/>
+      <c r="BE10" s="30"/>
+      <c r="BF10" s="30"/>
+      <c r="BG10" s="30"/>
+      <c r="BH10" s="30"/>
+      <c r="BI10" s="30"/>
+      <c r="BJ10" s="30"/>
+      <c r="BK10" s="30"/>
+      <c r="BL10" s="30"/>
+      <c r="BM10" s="30"/>
+      <c r="BN10" s="30"/>
+      <c r="BO10" s="30"/>
+      <c r="BP10" s="30"/>
+      <c r="BQ10" s="30"/>
+      <c r="BR10" s="30"/>
+      <c r="BS10" s="30"/>
+      <c r="BT10" s="30"/>
+      <c r="BU10" s="30"/>
+      <c r="BV10" s="30"/>
+      <c r="BW10" s="30"/>
+      <c r="BX10" s="30"/>
+      <c r="BY10" s="30"/>
+      <c r="BZ10" s="30"/>
+      <c r="CA10" s="30"/>
+      <c r="CB10" s="30"/>
+      <c r="CC10" s="30"/>
+      <c r="CD10" s="30"/>
+      <c r="CE10" s="30"/>
+      <c r="CF10" s="30"/>
+      <c r="CG10" s="30"/>
+      <c r="CH10" s="30"/>
+      <c r="CI10" s="30"/>
+      <c r="CJ10" s="30"/>
+      <c r="CK10" s="30"/>
+      <c r="CL10" s="30"/>
+      <c r="CM10" s="30"/>
+      <c r="CN10" s="30"/>
+      <c r="CO10" s="30"/>
+      <c r="CP10" s="30"/>
+      <c r="CQ10" s="30"/>
+      <c r="CR10" s="30"/>
+      <c r="CS10" s="30"/>
+      <c r="CT10" s="30"/>
+      <c r="CU10" s="30"/>
+      <c r="CV10" s="30"/>
+      <c r="CW10" s="30"/>
+      <c r="CX10" s="30"/>
+      <c r="CY10" s="30"/>
+      <c r="CZ10" s="30"/>
+      <c r="DA10" s="30"/>
+      <c r="DB10" s="30"/>
+      <c r="DC10" s="30"/>
+      <c r="DD10" s="30"/>
+      <c r="DE10" s="30"/>
+      <c r="DF10" s="30"/>
     </row>
     <row r="11" ht="45.0" customHeight="1">
-      <c r="A11" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="32"/>
-      <c r="AA11" s="32"/>
-      <c r="AB11" s="32"/>
-      <c r="AC11" s="32"/>
-      <c r="AD11" s="32"/>
-      <c r="AE11" s="32"/>
-      <c r="AF11" s="32"/>
-      <c r="AG11" s="32"/>
-      <c r="AH11" s="32"/>
-      <c r="AI11" s="32"/>
-      <c r="AJ11" s="32"/>
-      <c r="AK11" s="32"/>
-      <c r="AL11" s="32"/>
-      <c r="AM11" s="32"/>
-      <c r="AN11" s="32"/>
-      <c r="AO11" s="32"/>
-      <c r="AP11" s="32"/>
-      <c r="AQ11" s="32"/>
-      <c r="AR11" s="32"/>
-      <c r="AS11" s="32"/>
-      <c r="AT11" s="32"/>
-      <c r="AU11" s="32"/>
-      <c r="AV11" s="32"/>
-      <c r="AW11" s="32"/>
-      <c r="AX11" s="32"/>
-      <c r="AY11" s="32"/>
-      <c r="AZ11" s="32"/>
-      <c r="BA11" s="32"/>
-      <c r="BB11" s="32"/>
-      <c r="BC11" s="32"/>
-      <c r="BD11" s="32"/>
-      <c r="BE11" s="32"/>
-      <c r="BF11" s="32"/>
-      <c r="BG11" s="32"/>
-      <c r="BH11" s="32"/>
-      <c r="BI11" s="32"/>
-      <c r="BJ11" s="32"/>
-      <c r="BK11" s="32"/>
-      <c r="BL11" s="32"/>
-      <c r="BM11" s="32"/>
-      <c r="BN11" s="32"/>
-      <c r="BO11" s="32"/>
-      <c r="BP11" s="32"/>
-      <c r="BQ11" s="32"/>
-      <c r="BR11" s="32"/>
-      <c r="BS11" s="32"/>
-      <c r="BT11" s="32"/>
-      <c r="BU11" s="32"/>
-      <c r="BV11" s="32"/>
-      <c r="BW11" s="32"/>
-      <c r="BX11" s="32"/>
-      <c r="BY11" s="32"/>
-      <c r="BZ11" s="32"/>
-      <c r="CA11" s="32"/>
-      <c r="CB11" s="32"/>
-      <c r="CC11" s="32"/>
-      <c r="CD11" s="32"/>
-      <c r="CE11" s="32"/>
-      <c r="CF11" s="32"/>
-      <c r="CG11" s="32"/>
-      <c r="CH11" s="32"/>
-      <c r="CI11" s="32"/>
-      <c r="CJ11" s="32"/>
-      <c r="CK11" s="32"/>
-      <c r="CL11" s="32"/>
-      <c r="CM11" s="32"/>
-      <c r="CN11" s="32"/>
-      <c r="CO11" s="32"/>
-      <c r="CP11" s="32"/>
-      <c r="CQ11" s="32"/>
-      <c r="CR11" s="32"/>
-      <c r="CS11" s="32"/>
-      <c r="CT11" s="32"/>
-      <c r="CU11" s="32"/>
-      <c r="CV11" s="32"/>
-      <c r="CW11" s="32"/>
-      <c r="CX11" s="32"/>
-      <c r="CY11" s="32"/>
-      <c r="CZ11" s="32"/>
-      <c r="DA11" s="32"/>
-      <c r="DB11" s="32"/>
-      <c r="DC11" s="32"/>
+      <c r="A11" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="33"/>
+      <c r="AF11" s="33"/>
+      <c r="AG11" s="33"/>
+      <c r="AH11" s="33"/>
+      <c r="AI11" s="33"/>
+      <c r="AJ11" s="33"/>
+      <c r="AK11" s="33"/>
+      <c r="AL11" s="33"/>
+      <c r="AM11" s="33"/>
+      <c r="AN11" s="33"/>
+      <c r="AO11" s="33"/>
+      <c r="AP11" s="33"/>
+      <c r="AQ11" s="33"/>
+      <c r="AR11" s="33"/>
+      <c r="AS11" s="33"/>
+      <c r="AT11" s="33"/>
+      <c r="AU11" s="33"/>
+      <c r="AV11" s="33"/>
+      <c r="AW11" s="33"/>
+      <c r="AX11" s="33"/>
+      <c r="AY11" s="33"/>
+      <c r="AZ11" s="33"/>
+      <c r="BA11" s="33"/>
+      <c r="BB11" s="33"/>
+      <c r="BC11" s="33"/>
+      <c r="BD11" s="33"/>
+      <c r="BE11" s="33"/>
+      <c r="BF11" s="33"/>
+      <c r="BG11" s="33"/>
+      <c r="BH11" s="33"/>
+      <c r="BI11" s="33"/>
+      <c r="BJ11" s="33"/>
+      <c r="BK11" s="33"/>
+      <c r="BL11" s="33"/>
+      <c r="BM11" s="33"/>
+      <c r="BN11" s="33"/>
+      <c r="BO11" s="33"/>
+      <c r="BP11" s="33"/>
+      <c r="BQ11" s="33"/>
+      <c r="BR11" s="33"/>
+      <c r="BS11" s="33"/>
+      <c r="BT11" s="33"/>
+      <c r="BU11" s="33"/>
+      <c r="BV11" s="33"/>
+      <c r="BW11" s="33"/>
+      <c r="BX11" s="33"/>
+      <c r="BY11" s="33"/>
+      <c r="BZ11" s="33"/>
+      <c r="CA11" s="33"/>
+      <c r="CB11" s="33"/>
+      <c r="CC11" s="33"/>
+      <c r="CD11" s="33"/>
+      <c r="CE11" s="33"/>
+      <c r="CF11" s="33"/>
+      <c r="CG11" s="33"/>
+      <c r="CH11" s="33"/>
+      <c r="CI11" s="33"/>
+      <c r="CJ11" s="33"/>
+      <c r="CK11" s="33"/>
+      <c r="CL11" s="33"/>
+      <c r="CM11" s="33"/>
+      <c r="CN11" s="33"/>
+      <c r="CO11" s="33"/>
+      <c r="CP11" s="33"/>
+      <c r="CQ11" s="33"/>
+      <c r="CR11" s="33"/>
+      <c r="CS11" s="33"/>
+      <c r="CT11" s="33"/>
+      <c r="CU11" s="33"/>
+      <c r="CV11" s="33"/>
+      <c r="CW11" s="33"/>
+      <c r="CX11" s="33"/>
+      <c r="CY11" s="33"/>
+      <c r="CZ11" s="33"/>
+      <c r="DA11" s="33"/>
+      <c r="DB11" s="33"/>
+      <c r="DC11" s="33"/>
+      <c r="DD11" s="33"/>
+      <c r="DE11" s="33"/>
+      <c r="DF11" s="33"/>
     </row>
     <row r="12" ht="45.0" customHeight="1">
-      <c r="A12" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="29"/>
-      <c r="AC12" s="29"/>
-      <c r="AD12" s="29"/>
-      <c r="AE12" s="29"/>
-      <c r="AF12" s="29"/>
-      <c r="AG12" s="29"/>
-      <c r="AH12" s="29"/>
-      <c r="AI12" s="29"/>
-      <c r="AJ12" s="29"/>
-      <c r="AK12" s="29"/>
-      <c r="AL12" s="29"/>
-      <c r="AM12" s="29"/>
-      <c r="AN12" s="29"/>
-      <c r="AO12" s="29"/>
-      <c r="AP12" s="29"/>
-      <c r="AQ12" s="29"/>
-      <c r="AR12" s="29"/>
-      <c r="AS12" s="29"/>
-      <c r="AT12" s="29"/>
-      <c r="AU12" s="29"/>
-      <c r="AV12" s="29"/>
-      <c r="AW12" s="29"/>
-      <c r="AX12" s="29"/>
-      <c r="AY12" s="29"/>
-      <c r="AZ12" s="29"/>
-      <c r="BA12" s="29"/>
-      <c r="BB12" s="29"/>
-      <c r="BC12" s="29"/>
-      <c r="BD12" s="29"/>
-      <c r="BE12" s="29"/>
-      <c r="BF12" s="29"/>
-      <c r="BG12" s="29"/>
-      <c r="BH12" s="29"/>
-      <c r="BI12" s="29"/>
-      <c r="BJ12" s="29"/>
-      <c r="BK12" s="29"/>
-      <c r="BL12" s="29"/>
-      <c r="BM12" s="29"/>
-      <c r="BN12" s="29"/>
-      <c r="BO12" s="29"/>
-      <c r="BP12" s="29"/>
-      <c r="BQ12" s="29"/>
-      <c r="BR12" s="29"/>
-      <c r="BS12" s="29"/>
-      <c r="BT12" s="29"/>
-      <c r="BU12" s="29"/>
-      <c r="BV12" s="29"/>
-      <c r="BW12" s="29"/>
-      <c r="BX12" s="29"/>
-      <c r="BY12" s="29"/>
-      <c r="BZ12" s="29"/>
-      <c r="CA12" s="29"/>
-      <c r="CB12" s="29"/>
-      <c r="CC12" s="29"/>
-      <c r="CD12" s="29"/>
-      <c r="CE12" s="29"/>
-      <c r="CF12" s="29"/>
-      <c r="CG12" s="29"/>
-      <c r="CH12" s="29"/>
-      <c r="CI12" s="29"/>
-      <c r="CJ12" s="29"/>
-      <c r="CK12" s="29"/>
-      <c r="CL12" s="29"/>
-      <c r="CM12" s="29"/>
-      <c r="CN12" s="29"/>
-      <c r="CO12" s="29"/>
-      <c r="CP12" s="29"/>
-      <c r="CQ12" s="29"/>
-      <c r="CR12" s="29"/>
-      <c r="CS12" s="29"/>
-      <c r="CT12" s="29"/>
-      <c r="CU12" s="29"/>
-      <c r="CV12" s="29"/>
-      <c r="CW12" s="29"/>
-      <c r="CX12" s="29"/>
-      <c r="CY12" s="29"/>
-      <c r="CZ12" s="29"/>
-      <c r="DA12" s="29"/>
-      <c r="DB12" s="29"/>
-      <c r="DC12" s="29"/>
+      <c r="B12" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="30"/>
+      <c r="AD12" s="30"/>
+      <c r="AE12" s="30"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="30"/>
+      <c r="AI12" s="30"/>
+      <c r="AJ12" s="30"/>
+      <c r="AK12" s="30"/>
+      <c r="AL12" s="30"/>
+      <c r="AM12" s="30"/>
+      <c r="AN12" s="30"/>
+      <c r="AO12" s="30"/>
+      <c r="AP12" s="30"/>
+      <c r="AQ12" s="30"/>
+      <c r="AR12" s="30"/>
+      <c r="AS12" s="30"/>
+      <c r="AT12" s="30"/>
+      <c r="AU12" s="30"/>
+      <c r="AV12" s="30"/>
+      <c r="AW12" s="30"/>
+      <c r="AX12" s="30"/>
+      <c r="AY12" s="30"/>
+      <c r="AZ12" s="30"/>
+      <c r="BA12" s="30"/>
+      <c r="BB12" s="30"/>
+      <c r="BC12" s="30"/>
+      <c r="BD12" s="30"/>
+      <c r="BE12" s="30"/>
+      <c r="BF12" s="30"/>
+      <c r="BG12" s="30"/>
+      <c r="BH12" s="30"/>
+      <c r="BI12" s="30"/>
+      <c r="BJ12" s="30"/>
+      <c r="BK12" s="30"/>
+      <c r="BL12" s="30"/>
+      <c r="BM12" s="30"/>
+      <c r="BN12" s="30"/>
+      <c r="BO12" s="30"/>
+      <c r="BP12" s="30"/>
+      <c r="BQ12" s="30"/>
+      <c r="BR12" s="30"/>
+      <c r="BS12" s="30"/>
+      <c r="BT12" s="30"/>
+      <c r="BU12" s="30"/>
+      <c r="BV12" s="30"/>
+      <c r="BW12" s="30"/>
+      <c r="BX12" s="30"/>
+      <c r="BY12" s="30"/>
+      <c r="BZ12" s="30"/>
+      <c r="CA12" s="30"/>
+      <c r="CB12" s="30"/>
+      <c r="CC12" s="30"/>
+      <c r="CD12" s="30"/>
+      <c r="CE12" s="30"/>
+      <c r="CF12" s="30"/>
+      <c r="CG12" s="30"/>
+      <c r="CH12" s="30"/>
+      <c r="CI12" s="30"/>
+      <c r="CJ12" s="30"/>
+      <c r="CK12" s="30"/>
+      <c r="CL12" s="30"/>
+      <c r="CM12" s="30"/>
+      <c r="CN12" s="30"/>
+      <c r="CO12" s="30"/>
+      <c r="CP12" s="30"/>
+      <c r="CQ12" s="30"/>
+      <c r="CR12" s="30"/>
+      <c r="CS12" s="30"/>
+      <c r="CT12" s="30"/>
+      <c r="CU12" s="30"/>
+      <c r="CV12" s="30"/>
+      <c r="CW12" s="30"/>
+      <c r="CX12" s="30"/>
+      <c r="CY12" s="30"/>
+      <c r="CZ12" s="30"/>
+      <c r="DA12" s="30"/>
+      <c r="DB12" s="30"/>
+      <c r="DC12" s="30"/>
+      <c r="DD12" s="30"/>
+      <c r="DE12" s="30"/>
+      <c r="DF12" s="30"/>
     </row>
     <row r="13" ht="99.75" customHeight="1">
-      <c r="A13" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="31" t="s">
+      <c r="A13" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="32"/>
-      <c r="AC13" s="32"/>
-      <c r="AD13" s="32"/>
-      <c r="AE13" s="32"/>
-      <c r="AF13" s="32"/>
-      <c r="AG13" s="32"/>
-      <c r="AH13" s="32"/>
-      <c r="AI13" s="32"/>
-      <c r="AJ13" s="32"/>
-      <c r="AK13" s="32"/>
-      <c r="AL13" s="32"/>
-      <c r="AM13" s="32"/>
-      <c r="AN13" s="32"/>
-      <c r="AO13" s="32"/>
-      <c r="AP13" s="32"/>
-      <c r="AQ13" s="32"/>
-      <c r="AR13" s="32"/>
-      <c r="AS13" s="32"/>
-      <c r="AT13" s="32"/>
-      <c r="AU13" s="32"/>
-      <c r="AV13" s="32"/>
-      <c r="AW13" s="32"/>
-      <c r="AX13" s="32"/>
-      <c r="AY13" s="32"/>
-      <c r="AZ13" s="32"/>
-      <c r="BA13" s="32"/>
-      <c r="BB13" s="32"/>
-      <c r="BC13" s="32"/>
-      <c r="BD13" s="32"/>
-      <c r="BE13" s="32"/>
-      <c r="BF13" s="32"/>
-      <c r="BG13" s="32"/>
-      <c r="BH13" s="32"/>
-      <c r="BI13" s="32"/>
-      <c r="BJ13" s="32"/>
-      <c r="BK13" s="32"/>
-      <c r="BL13" s="32"/>
-      <c r="BM13" s="32"/>
-      <c r="BN13" s="32"/>
-      <c r="BO13" s="32"/>
-      <c r="BP13" s="32"/>
-      <c r="BQ13" s="32"/>
-      <c r="BR13" s="32"/>
-      <c r="BS13" s="32"/>
-      <c r="BT13" s="32"/>
-      <c r="BU13" s="32"/>
-      <c r="BV13" s="32"/>
-      <c r="BW13" s="32"/>
-      <c r="BX13" s="32"/>
-      <c r="BY13" s="32"/>
-      <c r="BZ13" s="32"/>
-      <c r="CA13" s="32"/>
-      <c r="CB13" s="32"/>
-      <c r="CC13" s="32"/>
-      <c r="CD13" s="32"/>
-      <c r="CE13" s="32"/>
-      <c r="CF13" s="32"/>
-      <c r="CG13" s="32"/>
-      <c r="CH13" s="32"/>
-      <c r="CI13" s="32"/>
-      <c r="CJ13" s="32"/>
-      <c r="CK13" s="32"/>
-      <c r="CL13" s="32"/>
-      <c r="CM13" s="32"/>
-      <c r="CN13" s="32"/>
-      <c r="CO13" s="32"/>
-      <c r="CP13" s="32"/>
-      <c r="CQ13" s="32"/>
-      <c r="CR13" s="32"/>
-      <c r="CS13" s="32"/>
-      <c r="CT13" s="32"/>
-      <c r="CU13" s="32"/>
-      <c r="CV13" s="32"/>
-      <c r="CW13" s="32"/>
-      <c r="CX13" s="32"/>
-      <c r="CY13" s="32"/>
-      <c r="CZ13" s="32"/>
-      <c r="DA13" s="32"/>
-      <c r="DB13" s="32"/>
-      <c r="DC13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="33"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="33"/>
+      <c r="AF13" s="33"/>
+      <c r="AG13" s="33"/>
+      <c r="AH13" s="33"/>
+      <c r="AI13" s="33"/>
+      <c r="AJ13" s="33"/>
+      <c r="AK13" s="33"/>
+      <c r="AL13" s="33"/>
+      <c r="AM13" s="33"/>
+      <c r="AN13" s="33"/>
+      <c r="AO13" s="33"/>
+      <c r="AP13" s="33"/>
+      <c r="AQ13" s="33"/>
+      <c r="AR13" s="33"/>
+      <c r="AS13" s="33"/>
+      <c r="AT13" s="33"/>
+      <c r="AU13" s="33"/>
+      <c r="AV13" s="33"/>
+      <c r="AW13" s="33"/>
+      <c r="AX13" s="33"/>
+      <c r="AY13" s="33"/>
+      <c r="AZ13" s="33"/>
+      <c r="BA13" s="33"/>
+      <c r="BB13" s="33"/>
+      <c r="BC13" s="33"/>
+      <c r="BD13" s="33"/>
+      <c r="BE13" s="33"/>
+      <c r="BF13" s="33"/>
+      <c r="BG13" s="33"/>
+      <c r="BH13" s="33"/>
+      <c r="BI13" s="33"/>
+      <c r="BJ13" s="33"/>
+      <c r="BK13" s="33"/>
+      <c r="BL13" s="33"/>
+      <c r="BM13" s="33"/>
+      <c r="BN13" s="33"/>
+      <c r="BO13" s="33"/>
+      <c r="BP13" s="33"/>
+      <c r="BQ13" s="33"/>
+      <c r="BR13" s="33"/>
+      <c r="BS13" s="33"/>
+      <c r="BT13" s="33"/>
+      <c r="BU13" s="33"/>
+      <c r="BV13" s="33"/>
+      <c r="BW13" s="33"/>
+      <c r="BX13" s="33"/>
+      <c r="BY13" s="33"/>
+      <c r="BZ13" s="33"/>
+      <c r="CA13" s="33"/>
+      <c r="CB13" s="33"/>
+      <c r="CC13" s="33"/>
+      <c r="CD13" s="33"/>
+      <c r="CE13" s="33"/>
+      <c r="CF13" s="33"/>
+      <c r="CG13" s="33"/>
+      <c r="CH13" s="33"/>
+      <c r="CI13" s="33"/>
+      <c r="CJ13" s="33"/>
+      <c r="CK13" s="33"/>
+      <c r="CL13" s="33"/>
+      <c r="CM13" s="33"/>
+      <c r="CN13" s="33"/>
+      <c r="CO13" s="33"/>
+      <c r="CP13" s="33"/>
+      <c r="CQ13" s="33"/>
+      <c r="CR13" s="33"/>
+      <c r="CS13" s="33"/>
+      <c r="CT13" s="33"/>
+      <c r="CU13" s="33"/>
+      <c r="CV13" s="33"/>
+      <c r="CW13" s="33"/>
+      <c r="CX13" s="33"/>
+      <c r="CY13" s="33"/>
+      <c r="CZ13" s="33"/>
+      <c r="DA13" s="33"/>
+      <c r="DB13" s="33"/>
+      <c r="DC13" s="33"/>
+      <c r="DD13" s="33"/>
+      <c r="DE13" s="33"/>
+      <c r="DF13" s="33"/>
     </row>
     <row r="14">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
-      <c r="AD14" s="26"/>
-      <c r="AE14" s="26"/>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
-      <c r="AH14" s="26"/>
-      <c r="AI14" s="26"/>
-      <c r="AJ14" s="26"/>
-      <c r="AK14" s="26"/>
-      <c r="AL14" s="26"/>
-      <c r="AM14" s="26"/>
-      <c r="AN14" s="26"/>
-      <c r="AO14" s="26"/>
-      <c r="AP14" s="26"/>
-      <c r="AQ14" s="26"/>
-      <c r="AR14" s="26"/>
-      <c r="AS14" s="26"/>
-      <c r="AT14" s="26"/>
-      <c r="AU14" s="26"/>
-      <c r="AV14" s="26"/>
-      <c r="AW14" s="26"/>
-      <c r="AX14" s="26"/>
-      <c r="AY14" s="26"/>
-      <c r="AZ14" s="26"/>
-      <c r="BA14" s="26"/>
-      <c r="BB14" s="26"/>
-      <c r="BC14" s="26"/>
-      <c r="BD14" s="26"/>
-      <c r="BE14" s="26"/>
-      <c r="BF14" s="26"/>
-      <c r="BG14" s="26"/>
-      <c r="BH14" s="26"/>
-      <c r="BI14" s="26"/>
-      <c r="BJ14" s="26"/>
-      <c r="BK14" s="26"/>
-      <c r="BL14" s="26"/>
-      <c r="BM14" s="26"/>
-      <c r="BN14" s="26"/>
-      <c r="BO14" s="26"/>
-      <c r="BP14" s="26"/>
-      <c r="BQ14" s="26"/>
-      <c r="BR14" s="26"/>
-      <c r="BS14" s="26"/>
-      <c r="BT14" s="26"/>
-      <c r="BU14" s="26"/>
-      <c r="BV14" s="26"/>
-      <c r="BW14" s="26"/>
-      <c r="BX14" s="26"/>
-      <c r="BY14" s="26"/>
-      <c r="BZ14" s="26"/>
-      <c r="CA14" s="26"/>
-      <c r="CB14" s="26"/>
-      <c r="CC14" s="26"/>
-      <c r="CD14" s="26"/>
-      <c r="CE14" s="26"/>
-      <c r="CF14" s="26"/>
-      <c r="CG14" s="26"/>
-      <c r="CH14" s="26"/>
-      <c r="CI14" s="26"/>
-      <c r="CJ14" s="26"/>
-      <c r="CK14" s="26"/>
-      <c r="CL14" s="26"/>
-      <c r="CM14" s="26"/>
-      <c r="CN14" s="26"/>
-      <c r="CO14" s="26"/>
-      <c r="CP14" s="26"/>
-      <c r="CQ14" s="26"/>
-      <c r="CR14" s="26"/>
-      <c r="CS14" s="26"/>
-      <c r="CT14" s="26"/>
-      <c r="CU14" s="26"/>
-      <c r="CV14" s="26"/>
-      <c r="CW14" s="26"/>
-      <c r="CX14" s="26"/>
-      <c r="CY14" s="26"/>
-      <c r="CZ14" s="26"/>
-      <c r="DA14" s="26"/>
-      <c r="DB14" s="26"/>
-      <c r="DC14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
+      <c r="AH14" s="27"/>
+      <c r="AI14" s="27"/>
+      <c r="AJ14" s="27"/>
+      <c r="AK14" s="27"/>
+      <c r="AL14" s="27"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="27"/>
+      <c r="AP14" s="27"/>
+      <c r="AQ14" s="27"/>
+      <c r="AR14" s="27"/>
+      <c r="AS14" s="27"/>
+      <c r="AT14" s="27"/>
+      <c r="AU14" s="27"/>
+      <c r="AV14" s="27"/>
+      <c r="AW14" s="27"/>
+      <c r="AX14" s="27"/>
+      <c r="AY14" s="27"/>
+      <c r="AZ14" s="27"/>
+      <c r="BA14" s="27"/>
+      <c r="BB14" s="27"/>
+      <c r="BC14" s="27"/>
+      <c r="BD14" s="27"/>
+      <c r="BE14" s="27"/>
+      <c r="BF14" s="27"/>
+      <c r="BG14" s="27"/>
+      <c r="BH14" s="27"/>
+      <c r="BI14" s="27"/>
+      <c r="BJ14" s="27"/>
+      <c r="BK14" s="27"/>
+      <c r="BL14" s="27"/>
+      <c r="BM14" s="27"/>
+      <c r="BN14" s="27"/>
+      <c r="BO14" s="27"/>
+      <c r="BP14" s="27"/>
+      <c r="BQ14" s="27"/>
+      <c r="BR14" s="27"/>
+      <c r="BS14" s="27"/>
+      <c r="BT14" s="27"/>
+      <c r="BU14" s="27"/>
+      <c r="BV14" s="27"/>
+      <c r="BW14" s="27"/>
+      <c r="BX14" s="27"/>
+      <c r="BY14" s="27"/>
+      <c r="BZ14" s="27"/>
+      <c r="CA14" s="27"/>
+      <c r="CB14" s="27"/>
+      <c r="CC14" s="27"/>
+      <c r="CD14" s="27"/>
+      <c r="CE14" s="27"/>
+      <c r="CF14" s="27"/>
+      <c r="CG14" s="27"/>
+      <c r="CH14" s="27"/>
+      <c r="CI14" s="27"/>
+      <c r="CJ14" s="27"/>
+      <c r="CK14" s="27"/>
+      <c r="CL14" s="27"/>
+      <c r="CM14" s="27"/>
+      <c r="CN14" s="27"/>
+      <c r="CO14" s="27"/>
+      <c r="CP14" s="27"/>
+      <c r="CQ14" s="27"/>
+      <c r="CR14" s="27"/>
+      <c r="CS14" s="27"/>
+      <c r="CT14" s="27"/>
+      <c r="CU14" s="27"/>
+      <c r="CV14" s="27"/>
+      <c r="CW14" s="27"/>
+      <c r="CX14" s="27"/>
+      <c r="CY14" s="27"/>
+      <c r="CZ14" s="27"/>
+      <c r="DA14" s="27"/>
+      <c r="DB14" s="27"/>
+      <c r="DC14" s="27"/>
+      <c r="DD14" s="27"/>
+      <c r="DE14" s="27"/>
+      <c r="DF14" s="27"/>
     </row>
     <row r="15" ht="75.0" customHeight="1">
-      <c r="A15" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="36"/>
-      <c r="AA15" s="36"/>
-      <c r="AB15" s="36"/>
-      <c r="AC15" s="36"/>
-      <c r="AD15" s="36"/>
-      <c r="AE15" s="36"/>
-      <c r="AF15" s="36"/>
-      <c r="AG15" s="36"/>
-      <c r="AH15" s="36"/>
-      <c r="AI15" s="36"/>
-      <c r="AJ15" s="36"/>
-      <c r="AK15" s="36"/>
-      <c r="AL15" s="36"/>
-      <c r="AM15" s="36"/>
-      <c r="AN15" s="36"/>
-      <c r="AO15" s="36"/>
-      <c r="AP15" s="36"/>
-      <c r="AQ15" s="36"/>
-      <c r="AR15" s="36"/>
-      <c r="AS15" s="36"/>
-      <c r="AT15" s="36"/>
-      <c r="AU15" s="36"/>
-      <c r="AV15" s="36"/>
-      <c r="AW15" s="36"/>
-      <c r="AX15" s="36"/>
-      <c r="AY15" s="36"/>
-      <c r="AZ15" s="36"/>
-      <c r="BA15" s="36"/>
-      <c r="BB15" s="36"/>
-      <c r="BC15" s="36"/>
-      <c r="BD15" s="36"/>
-      <c r="BE15" s="36"/>
-      <c r="BF15" s="36"/>
-      <c r="BG15" s="36"/>
-      <c r="BH15" s="36"/>
-      <c r="BI15" s="36"/>
-      <c r="BJ15" s="36"/>
-      <c r="BK15" s="36"/>
-      <c r="BL15" s="36"/>
-      <c r="BM15" s="36"/>
-      <c r="BN15" s="36"/>
-      <c r="BO15" s="36"/>
-      <c r="BP15" s="36"/>
-      <c r="BQ15" s="36"/>
-      <c r="BR15" s="36"/>
-      <c r="BS15" s="36"/>
-      <c r="BT15" s="36"/>
-      <c r="BU15" s="36"/>
-      <c r="BV15" s="36"/>
-      <c r="BW15" s="36"/>
-      <c r="BX15" s="36"/>
-      <c r="BY15" s="36"/>
-      <c r="BZ15" s="36"/>
-      <c r="CA15" s="36"/>
-      <c r="CB15" s="36"/>
-      <c r="CC15" s="36"/>
-      <c r="CD15" s="36"/>
-      <c r="CE15" s="36"/>
-      <c r="CF15" s="36"/>
-      <c r="CG15" s="36"/>
-      <c r="CH15" s="36"/>
-      <c r="CI15" s="36"/>
-      <c r="CJ15" s="36"/>
-      <c r="CK15" s="36"/>
-      <c r="CL15" s="36"/>
-      <c r="CM15" s="36"/>
-      <c r="CN15" s="36"/>
-      <c r="CO15" s="36"/>
-      <c r="CP15" s="36"/>
-      <c r="CQ15" s="36"/>
-      <c r="CR15" s="36"/>
-      <c r="CS15" s="36"/>
-      <c r="CT15" s="36"/>
-      <c r="CU15" s="36"/>
-      <c r="CV15" s="36"/>
-      <c r="CW15" s="36"/>
-      <c r="CX15" s="36"/>
-      <c r="CY15" s="36"/>
-      <c r="CZ15" s="36"/>
-      <c r="DA15" s="36"/>
-      <c r="DB15" s="36"/>
-      <c r="DC15" s="36"/>
+      <c r="A15" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+      <c r="Z15" s="37"/>
+      <c r="AA15" s="37"/>
+      <c r="AB15" s="37"/>
+      <c r="AC15" s="37"/>
+      <c r="AD15" s="37"/>
+      <c r="AE15" s="37"/>
+      <c r="AF15" s="37"/>
+      <c r="AG15" s="37"/>
+      <c r="AH15" s="37"/>
+      <c r="AI15" s="37"/>
+      <c r="AJ15" s="37"/>
+      <c r="AK15" s="37"/>
+      <c r="AL15" s="37"/>
+      <c r="AM15" s="37"/>
+      <c r="AN15" s="37"/>
+      <c r="AO15" s="37"/>
+      <c r="AP15" s="37"/>
+      <c r="AQ15" s="37"/>
+      <c r="AR15" s="37"/>
+      <c r="AS15" s="37"/>
+      <c r="AT15" s="37"/>
+      <c r="AU15" s="37"/>
+      <c r="AV15" s="37"/>
+      <c r="AW15" s="37"/>
+      <c r="AX15" s="37"/>
+      <c r="AY15" s="37"/>
+      <c r="AZ15" s="37"/>
+      <c r="BA15" s="37"/>
+      <c r="BB15" s="37"/>
+      <c r="BC15" s="37"/>
+      <c r="BD15" s="37"/>
+      <c r="BE15" s="37"/>
+      <c r="BF15" s="37"/>
+      <c r="BG15" s="37"/>
+      <c r="BH15" s="37"/>
+      <c r="BI15" s="37"/>
+      <c r="BJ15" s="37"/>
+      <c r="BK15" s="37"/>
+      <c r="BL15" s="37"/>
+      <c r="BM15" s="37"/>
+      <c r="BN15" s="37"/>
+      <c r="BO15" s="37"/>
+      <c r="BP15" s="37"/>
+      <c r="BQ15" s="37"/>
+      <c r="BR15" s="37"/>
+      <c r="BS15" s="37"/>
+      <c r="BT15" s="37"/>
+      <c r="BU15" s="37"/>
+      <c r="BV15" s="37"/>
+      <c r="BW15" s="37"/>
+      <c r="BX15" s="37"/>
+      <c r="BY15" s="37"/>
+      <c r="BZ15" s="37"/>
+      <c r="CA15" s="37"/>
+      <c r="CB15" s="37"/>
+      <c r="CC15" s="37"/>
+      <c r="CD15" s="37"/>
+      <c r="CE15" s="37"/>
+      <c r="CF15" s="37"/>
+      <c r="CG15" s="37"/>
+      <c r="CH15" s="37"/>
+      <c r="CI15" s="37"/>
+      <c r="CJ15" s="37"/>
+      <c r="CK15" s="37"/>
+      <c r="CL15" s="37"/>
+      <c r="CM15" s="37"/>
+      <c r="CN15" s="37"/>
+      <c r="CO15" s="37"/>
+      <c r="CP15" s="37"/>
+      <c r="CQ15" s="37"/>
+      <c r="CR15" s="37"/>
+      <c r="CS15" s="37"/>
+      <c r="CT15" s="37"/>
+      <c r="CU15" s="37"/>
+      <c r="CV15" s="37"/>
+      <c r="CW15" s="37"/>
+      <c r="CX15" s="37"/>
+      <c r="CY15" s="37"/>
+      <c r="CZ15" s="37"/>
+      <c r="DA15" s="37"/>
+      <c r="DB15" s="37"/>
+      <c r="DC15" s="37"/>
+      <c r="DD15" s="37"/>
+      <c r="DE15" s="37"/>
+      <c r="DF15" s="37"/>
     </row>
     <row r="16">
-      <c r="A16" s="37" t="s">
-        <v>131</v>
+      <c r="A16" s="38" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="38" t="s">
-        <v>132</v>
+      <c r="A17" s="39" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="15" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="39" t="s">
-        <v>134</v>
+      <c r="A19" s="40" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3978,7 +4046,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:DC1"/>
+    <mergeCell ref="A1:DF1"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>